<commit_message>
added more test cases to unit testing and integration testing in Excel and updated SDD
</commit_message>
<xml_diff>
--- a/Design/Testing_frame_work.xlsx
+++ b/Design/Testing_frame_work.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kathe\OneDrive\Desktop\Level_7\Business Application Programming\Assignment\Documation\Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kathe\ITPR7.508-Business-Application-Programming-Semester-One-2024\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA7D96F-7428-49B5-AA8B-6216E18E39FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5740F4B-94B6-46AB-8671-628F12D27FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_framwork_homeloanMointor" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="155">
   <si>
     <t>Status</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Unit Testing</t>
   </si>
   <si>
-    <t>Intergration Testing</t>
-  </si>
-  <si>
     <t xml:space="preserve">System Test </t>
   </si>
   <si>
@@ -167,9 +164,6 @@
     <t>integration with external systems</t>
   </si>
   <si>
-    <t>verify that the mortgage calculator application correctly interacts with the database to retrieve and store data, such as user information, loan details, and historical transactions.</t>
-  </si>
-  <si>
     <t>UT_mortgage_001</t>
   </si>
   <si>
@@ -308,24 +302,12 @@
     <t>input special characters or non-numeric values for numeric fields.</t>
   </si>
   <si>
-    <t>input invalid or out-of-range values for loan amount, interest rate, and loan term.</t>
-  </si>
-  <si>
-    <t>input negative values for loan amount or interest rate.</t>
-  </si>
-  <si>
     <t>calculate the mortgage payment for various loan scenarios with different input combinations</t>
   </si>
   <si>
-    <t>verify that user input from the interface such as loan amount, interest rate, and loan term is correctly passed to the calculation module.</t>
-  </si>
-  <si>
     <t>test generating an amortization schedule and verify that it accurately reflects the mortgage details. Such as principal balance, interest paid, remaining balance.</t>
   </si>
   <si>
-    <t>calculate the mortgage payment for a valid loan scenario such as $200,000 loan amount, 4% interest rate, 30-year term and verify the result.</t>
-  </si>
-  <si>
     <t>verify that the calculation module handles edge cases such as zero loan amount, zero interest rate, zero loan term.</t>
   </si>
   <si>
@@ -335,51 +317,9 @@
     <t>verify that the displayed mortgage payment is formatted correctly.</t>
   </si>
   <si>
-    <t>test the display of error messages if calculation errors occur.</t>
-  </si>
-  <si>
     <t>mock the external service response to simulate different scenarios such as successful response, error response.</t>
   </si>
   <si>
-    <t>test error handling and fallback mechanisms if the external service is unavailable or returns unexpected data.</t>
-  </si>
-  <si>
-    <t>IT_input_002</t>
-  </si>
-  <si>
-    <t>IT_input_003</t>
-  </si>
-  <si>
-    <t>IT_input_004</t>
-  </si>
-  <si>
-    <t>IT_input_005</t>
-  </si>
-  <si>
-    <t>IT_input_006</t>
-  </si>
-  <si>
-    <t>IT_input_007</t>
-  </si>
-  <si>
-    <t>IT_input_008</t>
-  </si>
-  <si>
-    <t>IT_input_009</t>
-  </si>
-  <si>
-    <t>IT_input_010</t>
-  </si>
-  <si>
-    <t>IT_input_011</t>
-  </si>
-  <si>
-    <t>IT_input_012</t>
-  </si>
-  <si>
-    <t>IT_calculation_002</t>
-  </si>
-  <si>
     <t>IT_calculation_003</t>
   </si>
   <si>
@@ -396,13 +336,175 @@
   </si>
   <si>
     <t>IT_external_003</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>Integration Testing</t>
+  </si>
+  <si>
+    <t>integration with authentication</t>
+  </si>
+  <si>
+    <t>ensure that only authenticated users can access the mortgage calculator functionality</t>
+  </si>
+  <si>
+    <t>navigation integration</t>
+  </si>
+  <si>
+    <t>form integration</t>
+  </si>
+  <si>
+    <t>performance Integration</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> test the performance of the webpage, including page load times, rendering speed, and resource utilization</t>
+  </si>
+  <si>
+    <t>layout integration</t>
+  </si>
+  <si>
+    <t>ensure that elements are positioned correctly</t>
+  </si>
+  <si>
+    <t>data retrieval integration</t>
+  </si>
+  <si>
+    <t>test the integration between the application and the database for retrieving data</t>
+  </si>
+  <si>
+    <t>verify that queries are executed correctly and return the expected results</t>
+  </si>
+  <si>
+    <t>test scenarios such as retrieving user information, loan details, and historical transactions</t>
+  </si>
+  <si>
+    <t>verifying that user input from the interface is correctly passed to the calculation module. This includes testing valid inputs, invalid inputs, and edge cases.</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>input invalid or out-of-range values for loan amount, and interest rate</t>
+  </si>
+  <si>
+    <t>UT_mortgage_009</t>
+  </si>
+  <si>
+    <t>UT_mortgage_010</t>
+  </si>
+  <si>
+    <t>UT_mortgage_011</t>
+  </si>
+  <si>
+    <t>UT_mortgage_012</t>
+  </si>
+  <si>
+    <t>UT_mortgage_013</t>
+  </si>
+  <si>
+    <t>UT_mortgage_014</t>
+  </si>
+  <si>
+    <t>UT_mortgage_015</t>
+  </si>
+  <si>
+    <t>UT_mortgage_016</t>
+  </si>
+  <si>
+    <t>UT_mortgage_017</t>
+  </si>
+  <si>
+    <t>UT_mortgage_018</t>
+  </si>
+  <si>
+    <t>test correct usernane and password for each users</t>
+  </si>
+  <si>
+    <t>test invalid credentials</t>
+  </si>
+  <si>
+    <t>test the navigation flow within the webpage, including links to different sections, buttons, and menus</t>
+  </si>
+  <si>
+    <t>ensure that users can navigate between pages or sections</t>
+  </si>
+  <si>
+    <t>verify that form fields are displayed correctly</t>
+  </si>
+  <si>
+    <t>validation messages appear when necessary</t>
+  </si>
+  <si>
+    <t>test the integration of forms within the webpage</t>
+  </si>
+  <si>
+    <t>form submissions are processed accurately</t>
+  </si>
+  <si>
+    <t>test error handling and fallback mechanisms if the external service is unavailable or returns unexpected data</t>
+  </si>
+  <si>
+    <t>verify that the mortgage calculator application correctly interacts with the database to retrieve and store data, such as user information, loan details, and historical transactions</t>
+  </si>
+  <si>
+    <t>test the display of error messages if calculation errors occur</t>
+  </si>
+  <si>
+    <t>error handling integration</t>
+  </si>
+  <si>
+    <t>verifying that appropriate error messages and fallback mechanisms are in place</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify that all API endpoints are accessible and return the correct HTTP status codes </t>
+  </si>
+  <si>
+    <t>GET request test</t>
+  </si>
+  <si>
+    <t>send a GET request to each endpoint and verify that the expected data is returned</t>
+  </si>
+  <si>
+    <t>POST Request test</t>
+  </si>
+  <si>
+    <t>endpoint availability test</t>
+  </si>
+  <si>
+    <t>verify that the resource is created successfully</t>
+  </si>
+  <si>
+    <t>PUT Request test</t>
+  </si>
+  <si>
+    <t>tests for both successful responses and error responses</t>
+  </si>
+  <si>
+    <t>verify that the resource is updated successfully</t>
+  </si>
+  <si>
+    <t>delete request test</t>
+  </si>
+  <si>
+    <t>verify that the resource is deleted successfully and that subsequent requests return a 404 status code for the deleted resource</t>
+  </si>
+  <si>
+    <t>test endpoints that require authentication by sending requests with valid and invalid authentication tokens.</t>
+  </si>
+  <si>
+    <t>verify that appropriate error responses such as 400 Bad Request are returned for invalid inputs.</t>
+  </si>
+  <si>
+    <t>include tests for valid input data, missing required fields, and invalid data formats.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -447,6 +549,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -468,7 +585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -514,11 +631,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
     <dxf>
       <font>
         <strike val="0"/>
@@ -528,24 +651,6 @@
         <vertAlign val="baseline"/>
         <sz val="14"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -611,6 +716,34 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -625,15 +758,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="B3:G79" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="B3:G79" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Testing Type" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test Area " dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Test scenario " dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Test ID" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Status" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Cause of test failure" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="B3:H113" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="B3:H113" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Testing Type" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test Area " dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Test scenario " dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Test ID" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Status" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Cause of test failure" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{A9217C57-AF58-4711-B17C-23BFFA04C7F1}" name="Column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -926,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:G94"/>
+  <dimension ref="A1:H128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="L56" sqref="L56"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -943,12 +1077,12 @@
     <col min="7" max="7" width="25" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="23.4">
+    <row r="1" spans="2:8" ht="23.4">
       <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="18">
+    <row r="3" spans="2:8" ht="18">
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
@@ -967,884 +1101,1338 @@
       <c r="G3" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" ht="18">
-      <c r="B4" s="16" t="s">
+      <c r="H3" s="17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="23.4">
+      <c r="B4" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="11"/>
       <c r="G4" s="12"/>
-    </row>
-    <row r="5" spans="2:7" ht="18">
+      <c r="H4" s="10"/>
+    </row>
+    <row r="5" spans="2:8" ht="18">
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="12"/>
-    </row>
-    <row r="6" spans="2:7" ht="18">
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" spans="2:8" ht="18">
       <c r="B6" s="9"/>
       <c r="C6" s="8"/>
       <c r="D6" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="12"/>
-    </row>
-    <row r="7" spans="2:7" ht="18">
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="2:8" ht="18">
       <c r="B7" s="9"/>
       <c r="C7" s="8"/>
       <c r="D7" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="12"/>
-    </row>
-    <row r="8" spans="2:7" ht="36">
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="2:8" ht="36">
       <c r="B8" s="9"/>
       <c r="C8" s="8"/>
       <c r="D8" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="2:7" ht="36">
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="2:8" ht="36">
       <c r="B9" s="9"/>
       <c r="C9" s="8"/>
       <c r="D9" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="12"/>
-    </row>
-    <row r="10" spans="2:7" ht="18">
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="2:8" ht="18">
       <c r="B10" s="9"/>
       <c r="C10" s="8"/>
       <c r="D10" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="12"/>
-    </row>
-    <row r="11" spans="2:7" ht="18">
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="2:8" ht="18">
       <c r="B11" s="9"/>
       <c r="C11" s="8"/>
       <c r="D11" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="12"/>
-    </row>
-    <row r="12" spans="2:7" ht="18">
+      <c r="H11" s="10"/>
+    </row>
+    <row r="12" spans="2:8" ht="18">
       <c r="B12" s="9"/>
       <c r="C12" s="8"/>
       <c r="D12" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="12"/>
-    </row>
-    <row r="13" spans="2:7" ht="18">
-      <c r="B13" s="9"/>
-      <c r="C13" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="10"/>
+      <c r="H12" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="18">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>118</v>
+      </c>
       <c r="F13" s="11"/>
       <c r="G13" s="12"/>
-    </row>
-    <row r="14" spans="2:7" ht="18">
+      <c r="H13" s="10"/>
+    </row>
+    <row r="14" spans="2:8" ht="18">
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="13" t="s">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>53</v>
+        <v>119</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="12"/>
-    </row>
-    <row r="15" spans="2:7" ht="18">
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
+      <c r="H14" s="10"/>
+    </row>
+    <row r="15" spans="2:8" ht="18">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
       <c r="D15" s="13" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>54</v>
+        <v>120</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="12"/>
-    </row>
-    <row r="16" spans="2:7" ht="18">
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
+      <c r="H15" s="10"/>
+    </row>
+    <row r="16" spans="2:8" ht="18">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
       <c r="D16" s="13" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>55</v>
+        <v>121</v>
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="12"/>
-    </row>
-    <row r="17" spans="2:7" ht="18">
-      <c r="B17" s="9"/>
+      <c r="H16" s="10"/>
+    </row>
+    <row r="17" spans="2:8" ht="18">
+      <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="13" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>56</v>
+        <v>122</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="2:7" ht="18">
-      <c r="B18" s="9"/>
+      <c r="H17" s="10"/>
+    </row>
+    <row r="18" spans="2:8" ht="18">
+      <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="13" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>57</v>
+        <v>123</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="12"/>
-    </row>
-    <row r="19" spans="2:7" ht="18">
-      <c r="B19" s="9"/>
-      <c r="C19" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="10"/>
+      <c r="H18" s="10"/>
+    </row>
+    <row r="19" spans="2:8" ht="18">
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>124</v>
+      </c>
       <c r="F19" s="11"/>
       <c r="G19" s="12"/>
-    </row>
-    <row r="20" spans="2:7" ht="18">
+      <c r="H19" s="10"/>
+    </row>
+    <row r="20" spans="2:8" ht="18">
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="13" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>58</v>
+        <v>125</v>
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="12"/>
-    </row>
-    <row r="21" spans="2:7" ht="36">
-      <c r="B21" s="9"/>
+      <c r="H20" s="10"/>
+    </row>
+    <row r="21" spans="2:8" ht="18">
+      <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="13" t="s">
-        <v>25</v>
+        <v>88</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>59</v>
+        <v>126</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="12"/>
-    </row>
-    <row r="22" spans="2:7" ht="18">
-      <c r="B22" s="9"/>
+      <c r="H21" s="10"/>
+    </row>
+    <row r="22" spans="2:8" ht="18">
+      <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="13" t="s">
-        <v>76</v>
+        <v>117</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>60</v>
+        <v>127</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="12"/>
-    </row>
-    <row r="23" spans="2:7" ht="18">
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>61</v>
-      </c>
+      <c r="H22" s="10"/>
+    </row>
+    <row r="23" spans="2:8" ht="18">
+      <c r="B23" s="9"/>
+      <c r="C23" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="10"/>
       <c r="F23" s="11"/>
       <c r="G23" s="12"/>
-    </row>
-    <row r="24" spans="2:7" ht="18">
+      <c r="H23" s="10"/>
+    </row>
+    <row r="24" spans="2:8" ht="18">
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="13" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F24" s="11"/>
       <c r="G24" s="12"/>
-    </row>
-    <row r="25" spans="2:7" ht="18">
+      <c r="H24" s="10"/>
+    </row>
+    <row r="25" spans="2:8" ht="18">
       <c r="B25" s="9"/>
-      <c r="C25" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="10"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="F25" s="11"/>
       <c r="G25" s="12"/>
-    </row>
-    <row r="26" spans="2:7" ht="36">
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
+      <c r="H25" s="10"/>
+    </row>
+    <row r="26" spans="2:8" ht="18">
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
       <c r="D26" s="13" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F26" s="11"/>
       <c r="G26" s="12"/>
-    </row>
-    <row r="27" spans="2:7" ht="18">
-      <c r="B27" s="8"/>
+      <c r="H26" s="10"/>
+    </row>
+    <row r="27" spans="2:8" ht="18">
+      <c r="B27" s="9"/>
       <c r="C27" s="8"/>
       <c r="D27" s="13" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="F27" s="11"/>
       <c r="G27" s="12"/>
-    </row>
-    <row r="28" spans="2:7" ht="18">
+      <c r="H27" s="10"/>
+    </row>
+    <row r="28" spans="2:8" ht="18">
       <c r="B28" s="9"/>
-      <c r="C28" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-    </row>
-    <row r="29" spans="2:7" ht="36">
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="F29" s="8"/>
-      <c r="G29" s="14"/>
-    </row>
-    <row r="30" spans="2:7" ht="18">
-      <c r="B30" s="9"/>
-      <c r="C30" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="14"/>
-    </row>
-    <row r="31" spans="2:7" ht="18">
-      <c r="B31" s="8"/>
-      <c r="C31" s="5"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" s="11"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="10"/>
+    </row>
+    <row r="29" spans="2:8" ht="18">
+      <c r="B29" s="9"/>
+      <c r="C29" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="13"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="10"/>
+    </row>
+    <row r="30" spans="2:8" ht="18">
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="11"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="10"/>
+    </row>
+    <row r="31" spans="2:8" ht="36">
+      <c r="B31" s="9"/>
+      <c r="C31" s="8"/>
       <c r="D31" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="F31" s="8"/>
-      <c r="G31" s="14"/>
-    </row>
-    <row r="32" spans="2:7" ht="18">
-      <c r="B32" s="8"/>
-      <c r="C32" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F31" s="11"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="10"/>
+    </row>
+    <row r="32" spans="2:8" ht="18">
+      <c r="B32" s="9"/>
+      <c r="C32" s="8"/>
       <c r="D32" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="F32" s="8"/>
-      <c r="G32" s="14"/>
-    </row>
-    <row r="33" spans="2:7" ht="18">
+        <v>74</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F32" s="11"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="10"/>
+    </row>
+    <row r="33" spans="1:8" ht="18">
       <c r="B33" s="8"/>
-      <c r="C33" s="5"/>
+      <c r="C33" s="8"/>
       <c r="D33" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F33" s="8"/>
-      <c r="G33" s="14"/>
-    </row>
-    <row r="34" spans="2:7" ht="18">
-      <c r="B34" s="9"/>
-      <c r="C34" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" s="13"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="14"/>
-    </row>
-    <row r="35" spans="2:7" ht="18">
-      <c r="B35" s="8"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F35" s="8"/>
-      <c r="G35" s="14"/>
-    </row>
-    <row r="36" spans="2:7" ht="18">
-      <c r="B36" s="9"/>
+        <v>25</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F33" s="11"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="10"/>
+    </row>
+    <row r="34" spans="1:8" ht="18">
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" s="11"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="10"/>
+    </row>
+    <row r="35" spans="1:8" ht="18">
+      <c r="B35" s="9"/>
+      <c r="C35" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="13"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="10"/>
+    </row>
+    <row r="36" spans="1:8" ht="36">
+      <c r="B36" s="8"/>
       <c r="C36" s="8"/>
       <c r="D36" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F36" s="8"/>
-      <c r="G36" s="14"/>
-    </row>
-    <row r="37" spans="2:7" ht="36">
+        <v>27</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F36" s="11"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="10"/>
+    </row>
+    <row r="37" spans="1:8" ht="18">
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
       <c r="D37" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F37" s="8"/>
-      <c r="G37" s="14"/>
-    </row>
-    <row r="38" spans="2:7" ht="20.25" customHeight="1">
-      <c r="B38" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="12"/>
-    </row>
-    <row r="39" spans="2:7" ht="20.25" customHeight="1">
+        <v>76</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37" s="11"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="10"/>
+    </row>
+    <row r="38" spans="1:8" ht="18">
+      <c r="B38" s="9"/>
+      <c r="C38" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="10"/>
+    </row>
+    <row r="39" spans="1:8" ht="36">
       <c r="B39" s="8"/>
-      <c r="C39" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D39" s="13"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="12"/>
-    </row>
-    <row r="40" spans="2:7" ht="20.25" customHeight="1">
-      <c r="B40" s="8"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F40" s="11"/>
-      <c r="G40" s="12"/>
-    </row>
-    <row r="41" spans="2:7" ht="20.25" customHeight="1">
+      <c r="C39" s="8"/>
+      <c r="D39" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F39" s="8"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="10"/>
+    </row>
+    <row r="40" spans="1:8" ht="18">
+      <c r="B40" s="9"/>
+      <c r="C40" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="13"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="10"/>
+    </row>
+    <row r="41" spans="1:8" ht="18">
       <c r="B41" s="8"/>
       <c r="C41" s="5"/>
       <c r="D41" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="F41" s="11"/>
-      <c r="G41" s="12"/>
-    </row>
-    <row r="42" spans="2:7" ht="20.25" customHeight="1">
+        <v>77</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F41" s="8"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="10"/>
+    </row>
+    <row r="42" spans="1:8" ht="18">
       <c r="B42" s="8"/>
       <c r="C42" s="5"/>
       <c r="D42" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="F42" s="11"/>
-      <c r="G42" s="12"/>
-    </row>
-    <row r="43" spans="2:7" ht="20.25" customHeight="1">
+        <v>28</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F42" s="8"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="10"/>
+    </row>
+    <row r="43" spans="1:8" ht="18">
       <c r="B43" s="8"/>
       <c r="C43" s="5"/>
       <c r="D43" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="F43" s="11"/>
-      <c r="G43" s="12"/>
-    </row>
-    <row r="44" spans="2:7" ht="20.25" customHeight="1">
-      <c r="B44" s="8"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="F44" s="11"/>
-      <c r="G44" s="12"/>
-    </row>
-    <row r="45" spans="2:7" ht="20.25" customHeight="1">
+        <v>78</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F43" s="8"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="10"/>
+    </row>
+    <row r="44" spans="1:8" ht="18">
+      <c r="B44" s="9"/>
+      <c r="C44" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="13"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="10"/>
+    </row>
+    <row r="45" spans="1:8" ht="18">
       <c r="B45" s="8"/>
       <c r="C45" s="5"/>
       <c r="D45" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="F45" s="11"/>
-      <c r="G45" s="12"/>
-    </row>
-    <row r="46" spans="2:7" ht="20.25" customHeight="1">
-      <c r="B46" s="8"/>
-      <c r="C46" s="5"/>
+        <v>79</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F45" s="8"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="10"/>
+    </row>
+    <row r="46" spans="1:8" ht="18">
+      <c r="B46" s="9"/>
+      <c r="C46" s="8"/>
       <c r="D46" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="F46" s="11"/>
-      <c r="G46" s="12"/>
-    </row>
-    <row r="47" spans="2:7" ht="20.25" customHeight="1">
+        <v>29</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F46" s="8"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="10"/>
+    </row>
+    <row r="47" spans="1:8" ht="36">
       <c r="B47" s="8"/>
-      <c r="C47" s="5"/>
+      <c r="C47" s="8"/>
       <c r="D47" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="F47" s="11"/>
-      <c r="G47" s="12"/>
-    </row>
-    <row r="48" spans="2:7" ht="20.25" customHeight="1">
-      <c r="B48" s="8"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>110</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F47" s="8"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="10"/>
+    </row>
+    <row r="48" spans="1:8" ht="20.25" customHeight="1">
+      <c r="A48" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C48" s="8"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
       <c r="F48" s="11"/>
       <c r="G48" s="12"/>
-    </row>
-    <row r="49" spans="2:7" ht="20.25" customHeight="1">
+      <c r="H48" s="10"/>
+    </row>
+    <row r="49" spans="2:8" ht="20.25" customHeight="1">
       <c r="B49" s="8"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>111</v>
-      </c>
+      <c r="C49" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D49" s="13"/>
+      <c r="E49" s="10"/>
       <c r="F49" s="11"/>
       <c r="G49" s="12"/>
-    </row>
-    <row r="50" spans="2:7" ht="20.25" customHeight="1">
+      <c r="H49" s="10"/>
+    </row>
+    <row r="50" spans="2:8" ht="20.25" customHeight="1">
       <c r="B50" s="8"/>
       <c r="C50" s="5"/>
       <c r="D50" s="13" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>112</v>
+        <v>70</v>
       </c>
       <c r="F50" s="11"/>
       <c r="G50" s="12"/>
-    </row>
-    <row r="51" spans="2:7" ht="20.25" customHeight="1">
+      <c r="H50" s="10"/>
+    </row>
+    <row r="51" spans="2:8" ht="20.25" customHeight="1">
       <c r="B51" s="8"/>
       <c r="C51" s="5"/>
       <c r="D51" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="E51" s="10" t="s">
-        <v>113</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="E51" s="10"/>
       <c r="F51" s="11"/>
       <c r="G51" s="12"/>
-    </row>
-    <row r="52" spans="2:7" ht="20.25" customHeight="1">
+      <c r="H51" s="10"/>
+    </row>
+    <row r="52" spans="2:8" ht="20.25" customHeight="1">
       <c r="B52" s="8"/>
-      <c r="C52" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D52" s="13"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="13" t="s">
+        <v>154</v>
+      </c>
       <c r="E52" s="10"/>
       <c r="F52" s="11"/>
       <c r="G52" s="12"/>
-    </row>
-    <row r="53" spans="2:7" ht="20.25" customHeight="1">
+      <c r="H52" s="10"/>
+    </row>
+    <row r="53" spans="2:8" ht="20.25" customHeight="1">
       <c r="B53" s="8"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E53" s="10" t="s">
-        <v>73</v>
-      </c>
+      <c r="C53" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D53" s="13"/>
+      <c r="E53" s="10"/>
       <c r="F53" s="11"/>
       <c r="G53" s="12"/>
-    </row>
-    <row r="54" spans="2:7" ht="20.25" customHeight="1">
+      <c r="H53" s="10"/>
+    </row>
+    <row r="54" spans="2:8" ht="20.25" customHeight="1">
       <c r="B54" s="8"/>
       <c r="C54" s="5"/>
       <c r="D54" s="13" t="s">
-        <v>96</v>
+        <v>37</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>114</v>
+        <v>71</v>
       </c>
       <c r="F54" s="11"/>
       <c r="G54" s="12"/>
-    </row>
-    <row r="55" spans="2:7" ht="20.25" customHeight="1">
+      <c r="H54" s="10"/>
+    </row>
+    <row r="55" spans="2:8" ht="20.25" customHeight="1">
       <c r="B55" s="8"/>
       <c r="C55" s="5"/>
       <c r="D55" s="13" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="F55" s="11"/>
       <c r="G55" s="12"/>
-    </row>
-    <row r="56" spans="2:7" ht="20.25" customHeight="1">
+      <c r="H55" s="10"/>
+    </row>
+    <row r="56" spans="2:8" ht="20.25" customHeight="1">
       <c r="B56" s="8"/>
       <c r="C56" s="5"/>
       <c r="D56" s="13" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="F56" s="11"/>
       <c r="G56" s="12"/>
-    </row>
-    <row r="57" spans="2:7" ht="20.25" customHeight="1">
+      <c r="H56" s="10"/>
+    </row>
+    <row r="57" spans="2:8" ht="20.25" customHeight="1">
       <c r="B57" s="8"/>
       <c r="C57" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D57" s="13"/>
       <c r="E57" s="10"/>
       <c r="F57" s="11"/>
       <c r="G57" s="12"/>
-    </row>
-    <row r="58" spans="2:7" ht="20.25" customHeight="1">
+      <c r="H57" s="10"/>
+    </row>
+    <row r="58" spans="2:8" ht="20.25" customHeight="1">
       <c r="B58" s="8"/>
       <c r="C58" s="5"/>
       <c r="D58" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F58" s="11"/>
       <c r="G58" s="12"/>
-    </row>
-    <row r="59" spans="2:7" ht="20.25" customHeight="1">
+      <c r="H58" s="10"/>
+    </row>
+    <row r="59" spans="2:8" ht="20.25" customHeight="1">
       <c r="B59" s="8"/>
       <c r="C59" s="5"/>
       <c r="D59" s="13" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="F59" s="11"/>
       <c r="G59" s="12"/>
-    </row>
-    <row r="60" spans="2:7" ht="20.25" customHeight="1">
+      <c r="H59" s="10"/>
+    </row>
+    <row r="60" spans="2:8" ht="20.25" customHeight="1">
       <c r="B60" s="8"/>
       <c r="C60" s="5"/>
       <c r="D60" s="13" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="F60" s="11"/>
       <c r="G60" s="12"/>
-    </row>
-    <row r="61" spans="2:7" ht="20.25" customHeight="1">
+      <c r="H60" s="10"/>
+    </row>
+    <row r="61" spans="2:8" ht="20.25" customHeight="1">
       <c r="B61" s="8"/>
       <c r="C61" s="5"/>
       <c r="D61" s="13" t="s">
-        <v>100</v>
+        <v>138</v>
       </c>
       <c r="E61" s="10"/>
       <c r="F61" s="11"/>
       <c r="G61" s="12"/>
-    </row>
-    <row r="62" spans="2:7" ht="20.25" customHeight="1">
+      <c r="H61" s="10"/>
+    </row>
+    <row r="62" spans="2:8" ht="20.25" customHeight="1">
       <c r="B62" s="8"/>
       <c r="C62" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D62" s="13"/>
       <c r="E62" s="10"/>
       <c r="F62" s="11"/>
       <c r="G62" s="12"/>
-    </row>
-    <row r="63" spans="2:7" ht="20.25" customHeight="1">
+      <c r="H62" s="10"/>
+    </row>
+    <row r="63" spans="2:8" ht="20.25" customHeight="1">
       <c r="B63" s="8"/>
       <c r="C63" s="5"/>
       <c r="D63" s="13" t="s">
-        <v>44</v>
+        <v>137</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F63" s="11"/>
       <c r="G63" s="12"/>
-    </row>
-    <row r="64" spans="2:7" ht="20.25" customHeight="1">
+      <c r="H63" s="10"/>
+    </row>
+    <row r="64" spans="2:8" ht="20.25" customHeight="1">
       <c r="B64" s="8"/>
       <c r="C64" s="5"/>
       <c r="D64" s="13" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="F64" s="11"/>
       <c r="G64" s="12"/>
-    </row>
-    <row r="65" spans="2:7" ht="20.25" customHeight="1">
+      <c r="H64" s="10"/>
+    </row>
+    <row r="65" spans="2:8" ht="20.25" customHeight="1">
       <c r="B65" s="8"/>
       <c r="C65" s="5"/>
       <c r="D65" s="13" t="s">
-        <v>102</v>
+        <v>136</v>
       </c>
       <c r="E65" s="10" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="F65" s="11"/>
       <c r="G65" s="12"/>
-    </row>
-    <row r="66" spans="2:7" ht="18">
-      <c r="B66" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C66" s="8"/>
-      <c r="D66" s="10"/>
+      <c r="H65" s="10"/>
+    </row>
+    <row r="66" spans="2:8" ht="20.25" customHeight="1">
+      <c r="B66" s="8"/>
+      <c r="C66" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D66" s="13"/>
       <c r="E66" s="10"/>
       <c r="F66" s="11"/>
-      <c r="G66" s="15"/>
-    </row>
-    <row r="67" spans="2:7" ht="18">
-      <c r="B67" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C67" s="8"/>
-      <c r="D67" s="13"/>
+      <c r="G66" s="12"/>
+      <c r="H66" s="10"/>
+    </row>
+    <row r="67" spans="2:8" ht="20.25" customHeight="1">
+      <c r="B67" s="8"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="13" t="s">
+        <v>104</v>
+      </c>
       <c r="E67" s="10"/>
       <c r="F67" s="11"/>
-      <c r="G67" s="15"/>
-    </row>
-    <row r="68" spans="2:7" ht="18">
+      <c r="G67" s="12"/>
+      <c r="H67" s="10"/>
+    </row>
+    <row r="68" spans="2:8" ht="20.25" customHeight="1">
       <c r="B68" s="8"/>
-      <c r="C68" s="8"/>
-      <c r="D68" s="8"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="13" t="s">
+        <v>128</v>
+      </c>
       <c r="E68" s="10"/>
       <c r="F68" s="11"/>
-      <c r="G68" s="15"/>
-    </row>
-    <row r="69" spans="2:7" ht="18">
+      <c r="G68" s="12"/>
+      <c r="H68" s="10"/>
+    </row>
+    <row r="69" spans="2:8" ht="20.25" customHeight="1">
       <c r="B69" s="8"/>
-      <c r="C69" s="8"/>
-      <c r="D69" s="8"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="13" t="s">
+        <v>129</v>
+      </c>
       <c r="E69" s="10"/>
       <c r="F69" s="11"/>
-      <c r="G69" s="15"/>
-    </row>
-    <row r="70" spans="2:7" ht="18">
+      <c r="G69" s="12"/>
+      <c r="H69" s="10"/>
+    </row>
+    <row r="70" spans="2:8" ht="20.25" customHeight="1">
       <c r="B70" s="8"/>
-      <c r="C70" s="8"/>
-      <c r="D70" s="8"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="13" t="s">
+        <v>152</v>
+      </c>
       <c r="E70" s="10"/>
       <c r="F70" s="11"/>
-      <c r="G70" s="15"/>
-    </row>
-    <row r="71" spans="2:7" ht="18">
+      <c r="G70" s="12"/>
+      <c r="H70" s="10"/>
+    </row>
+    <row r="71" spans="2:8" ht="20.25" customHeight="1">
       <c r="B71" s="8"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="8"/>
+      <c r="C71" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D71" s="13"/>
       <c r="E71" s="10"/>
       <c r="F71" s="11"/>
-      <c r="G71" s="15"/>
-    </row>
-    <row r="72" spans="2:7" ht="18">
+      <c r="G71" s="12"/>
+      <c r="H71" s="10"/>
+    </row>
+    <row r="72" spans="2:8" ht="20.25" customHeight="1">
       <c r="B72" s="8"/>
-      <c r="C72" s="8"/>
-      <c r="D72" s="8"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="13" t="s">
+        <v>130</v>
+      </c>
       <c r="E72" s="10"/>
       <c r="F72" s="11"/>
-      <c r="G72" s="15"/>
-    </row>
-    <row r="73" spans="2:7" ht="18">
+      <c r="G72" s="12"/>
+      <c r="H72" s="10"/>
+    </row>
+    <row r="73" spans="2:8" ht="20.25" customHeight="1">
       <c r="B73" s="8"/>
-      <c r="C73" s="8"/>
-      <c r="D73" s="10"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="13" t="s">
+        <v>131</v>
+      </c>
       <c r="E73" s="10"/>
       <c r="F73" s="11"/>
-      <c r="G73" s="15"/>
-    </row>
-    <row r="74" spans="2:7" ht="18">
+      <c r="G73" s="12"/>
+      <c r="H73" s="10"/>
+    </row>
+    <row r="74" spans="2:8" ht="20.25" customHeight="1">
       <c r="B74" s="8"/>
-      <c r="C74" s="8"/>
-      <c r="D74" s="10"/>
+      <c r="C74" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="D74" s="13"/>
       <c r="E74" s="10"/>
       <c r="F74" s="11"/>
-      <c r="G74" s="15"/>
-    </row>
-    <row r="75" spans="2:7" ht="18">
+      <c r="G74" s="12"/>
+      <c r="H74" s="10"/>
+    </row>
+    <row r="75" spans="2:8" ht="20.25" customHeight="1">
       <c r="B75" s="8"/>
-      <c r="C75" s="8"/>
-      <c r="D75" s="10"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="13" t="s">
+        <v>134</v>
+      </c>
       <c r="E75" s="10"/>
       <c r="F75" s="11"/>
-      <c r="G75" s="15"/>
-    </row>
-    <row r="76" spans="2:7" ht="18">
+      <c r="G75" s="12"/>
+      <c r="H75" s="10"/>
+    </row>
+    <row r="76" spans="2:8" ht="20.25" customHeight="1">
       <c r="B76" s="8"/>
-      <c r="C76" s="8"/>
-      <c r="D76" s="10"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="13" t="s">
+        <v>133</v>
+      </c>
       <c r="E76" s="10"/>
       <c r="F76" s="11"/>
-      <c r="G76" s="15"/>
-    </row>
-    <row r="77" spans="2:7" ht="18">
+      <c r="G76" s="12"/>
+      <c r="H76" s="10"/>
+    </row>
+    <row r="77" spans="2:8" ht="19.8" customHeight="1">
       <c r="B77" s="8"/>
-      <c r="C77" s="8"/>
-      <c r="D77" s="10"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="13" t="s">
+        <v>132</v>
+      </c>
       <c r="E77" s="10"/>
       <c r="F77" s="11"/>
-      <c r="G77" s="15"/>
-    </row>
-    <row r="78" spans="2:7" ht="18">
+      <c r="G77" s="12"/>
+      <c r="H77" s="10"/>
+    </row>
+    <row r="78" spans="2:8" ht="19.8" customHeight="1">
       <c r="B78" s="8"/>
-      <c r="C78" s="8"/>
-      <c r="D78" s="10"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="13" t="s">
+        <v>135</v>
+      </c>
       <c r="E78" s="10"/>
       <c r="F78" s="11"/>
-      <c r="G78" s="15"/>
-    </row>
-    <row r="79" spans="2:7" ht="18">
+      <c r="G78" s="12"/>
+      <c r="H78" s="10"/>
+    </row>
+    <row r="79" spans="2:8" ht="20.25" customHeight="1">
       <c r="B79" s="8"/>
-      <c r="C79" s="8"/>
-      <c r="D79" s="10"/>
+      <c r="C79" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D79" s="13"/>
       <c r="E79" s="10"/>
       <c r="F79" s="11"/>
       <c r="G79" s="12"/>
-    </row>
-    <row r="84" spans="3:4">
-      <c r="C84" s="2"/>
-      <c r="D84"/>
-    </row>
-    <row r="85" spans="3:4">
-      <c r="C85" s="2"/>
-      <c r="D85"/>
-    </row>
-    <row r="86" spans="3:4">
-      <c r="C86" s="2"/>
-      <c r="D86"/>
-    </row>
-    <row r="87" spans="3:4">
-      <c r="C87" s="2"/>
-      <c r="D87"/>
-    </row>
-    <row r="88" spans="3:4">
-      <c r="C88" s="2"/>
-      <c r="D88"/>
-    </row>
-    <row r="89" spans="3:4">
-      <c r="C89" s="2"/>
-      <c r="D89"/>
-    </row>
-    <row r="90" spans="3:4">
-      <c r="C90" s="2"/>
-      <c r="D90"/>
-    </row>
-    <row r="91" spans="3:4">
-      <c r="C91" s="2"/>
-      <c r="D91"/>
-    </row>
-    <row r="92" spans="3:4">
-      <c r="C92" s="2"/>
-      <c r="D92"/>
-    </row>
-    <row r="93" spans="3:4">
-      <c r="C93" s="2"/>
-    </row>
-    <row r="94" spans="3:4">
-      <c r="C94" s="2"/>
+      <c r="H79" s="10"/>
+    </row>
+    <row r="80" spans="2:8" ht="20.25" customHeight="1">
+      <c r="B80" s="8"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E80" s="10"/>
+      <c r="F80" s="11"/>
+      <c r="G80" s="12"/>
+      <c r="H80" s="10"/>
+    </row>
+    <row r="81" spans="2:8" ht="19.8" customHeight="1">
+      <c r="B81" s="8"/>
+      <c r="C81" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="D81" s="13"/>
+      <c r="E81" s="10"/>
+      <c r="F81" s="11"/>
+      <c r="G81" s="12"/>
+      <c r="H81" s="10"/>
+    </row>
+    <row r="82" spans="2:8" ht="19.8" customHeight="1">
+      <c r="B82" s="8"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="E82" s="10"/>
+      <c r="F82" s="11"/>
+      <c r="G82" s="12"/>
+      <c r="H82" s="10"/>
+    </row>
+    <row r="83" spans="2:8" ht="19.8" customHeight="1">
+      <c r="B83" s="8"/>
+      <c r="C83" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D83" s="13"/>
+      <c r="E83" s="10"/>
+      <c r="F83" s="11"/>
+      <c r="G83" s="12"/>
+      <c r="H83" s="10"/>
+    </row>
+    <row r="84" spans="2:8" ht="19.8" customHeight="1">
+      <c r="B84" s="8"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="E84" s="10"/>
+      <c r="F84" s="11"/>
+      <c r="G84" s="12"/>
+      <c r="H84" s="10"/>
+    </row>
+    <row r="85" spans="2:8" ht="19.8" customHeight="1">
+      <c r="B85" s="8"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E85" s="10"/>
+      <c r="F85" s="11"/>
+      <c r="G85" s="12"/>
+      <c r="H85" s="10"/>
+    </row>
+    <row r="86" spans="2:8" ht="19.8" customHeight="1">
+      <c r="B86" s="8"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E86" s="10"/>
+      <c r="F86" s="11"/>
+      <c r="G86" s="12"/>
+      <c r="H86" s="10"/>
+    </row>
+    <row r="87" spans="2:8" ht="19.8" customHeight="1">
+      <c r="B87" s="8"/>
+      <c r="C87" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D87" s="13"/>
+      <c r="E87" s="10"/>
+      <c r="F87" s="11"/>
+      <c r="G87" s="12"/>
+      <c r="H87" s="10"/>
+    </row>
+    <row r="88" spans="2:8" ht="19.8" customHeight="1">
+      <c r="B88" s="8"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="E88" s="10"/>
+      <c r="F88" s="11"/>
+      <c r="G88" s="12"/>
+      <c r="H88" s="10"/>
+    </row>
+    <row r="89" spans="2:8" ht="19.8" customHeight="1">
+      <c r="B89" s="8"/>
+      <c r="C89" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="D89" s="13"/>
+      <c r="E89" s="10"/>
+      <c r="F89" s="11"/>
+      <c r="G89" s="12"/>
+      <c r="H89" s="10"/>
+    </row>
+    <row r="90" spans="2:8" ht="19.8" customHeight="1">
+      <c r="B90" s="8"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="E90" s="10"/>
+      <c r="F90" s="11"/>
+      <c r="G90" s="12"/>
+      <c r="H90" s="10"/>
+    </row>
+    <row r="91" spans="2:8" ht="19.8" customHeight="1">
+      <c r="B91" s="8"/>
+      <c r="C91" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="D91" s="13"/>
+      <c r="E91" s="10"/>
+      <c r="F91" s="11"/>
+      <c r="G91" s="12"/>
+      <c r="H91" s="10"/>
+    </row>
+    <row r="92" spans="2:8" ht="19.8" customHeight="1">
+      <c r="B92" s="8"/>
+      <c r="C92" s="5"/>
+      <c r="D92" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="E92" s="10"/>
+      <c r="F92" s="11"/>
+      <c r="G92" s="12"/>
+      <c r="H92" s="10"/>
+    </row>
+    <row r="93" spans="2:8" ht="19.8" customHeight="1">
+      <c r="B93" s="8"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E93" s="10"/>
+      <c r="F93" s="11"/>
+      <c r="G93" s="12"/>
+      <c r="H93" s="10"/>
+    </row>
+    <row r="94" spans="2:8" ht="19.8" customHeight="1">
+      <c r="B94" s="8"/>
+      <c r="C94" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D94" s="13"/>
+      <c r="E94" s="10"/>
+      <c r="F94" s="11"/>
+      <c r="G94" s="12"/>
+      <c r="H94" s="10"/>
+    </row>
+    <row r="95" spans="2:8" ht="19.8" customHeight="1">
+      <c r="B95" s="8"/>
+      <c r="C95" s="5"/>
+      <c r="D95" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="E95" s="10"/>
+      <c r="F95" s="11"/>
+      <c r="G95" s="12"/>
+      <c r="H95" s="10"/>
+    </row>
+    <row r="96" spans="2:8" ht="19.8" customHeight="1">
+      <c r="B96" s="8"/>
+      <c r="C96" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="D96" s="13"/>
+      <c r="E96" s="10"/>
+      <c r="F96" s="11"/>
+      <c r="G96" s="12"/>
+      <c r="H96" s="10"/>
+    </row>
+    <row r="97" spans="2:8" ht="19.8" customHeight="1">
+      <c r="B97" s="8"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="E97" s="10"/>
+      <c r="F97" s="11"/>
+      <c r="G97" s="12"/>
+      <c r="H97" s="10"/>
+    </row>
+    <row r="98" spans="2:8" ht="19.8" customHeight="1">
+      <c r="B98" s="8"/>
+      <c r="C98" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="D98" s="13"/>
+      <c r="E98" s="10"/>
+      <c r="F98" s="11"/>
+      <c r="G98" s="12"/>
+      <c r="H98" s="10"/>
+    </row>
+    <row r="99" spans="2:8" ht="19.8" customHeight="1">
+      <c r="B99" s="8"/>
+      <c r="C99" s="5"/>
+      <c r="D99" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="E99" s="10"/>
+      <c r="F99" s="11"/>
+      <c r="G99" s="12"/>
+      <c r="H99" s="10"/>
+    </row>
+    <row r="100" spans="2:8" ht="18">
+      <c r="B100" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C100" s="8"/>
+      <c r="D100" s="10"/>
+      <c r="E100" s="10"/>
+      <c r="F100" s="11"/>
+      <c r="G100" s="15"/>
+      <c r="H100" s="10"/>
+    </row>
+    <row r="101" spans="2:8" ht="18">
+      <c r="B101" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C101" s="8"/>
+      <c r="D101" s="13"/>
+      <c r="E101" s="10"/>
+      <c r="F101" s="11"/>
+      <c r="G101" s="15"/>
+      <c r="H101" s="10"/>
+    </row>
+    <row r="102" spans="2:8" ht="18">
+      <c r="B102" s="8"/>
+      <c r="C102" s="8"/>
+      <c r="D102" s="8"/>
+      <c r="E102" s="10"/>
+      <c r="F102" s="11"/>
+      <c r="G102" s="15"/>
+      <c r="H102" s="10"/>
+    </row>
+    <row r="103" spans="2:8" ht="18">
+      <c r="B103" s="8"/>
+      <c r="C103" s="8"/>
+      <c r="D103" s="8"/>
+      <c r="E103" s="10"/>
+      <c r="F103" s="11"/>
+      <c r="G103" s="15"/>
+      <c r="H103" s="10"/>
+    </row>
+    <row r="104" spans="2:8" ht="18">
+      <c r="B104" s="8"/>
+      <c r="C104" s="8"/>
+      <c r="D104" s="8"/>
+      <c r="E104" s="10"/>
+      <c r="F104" s="11"/>
+      <c r="G104" s="15"/>
+      <c r="H104" s="10"/>
+    </row>
+    <row r="105" spans="2:8" ht="18">
+      <c r="B105" s="8"/>
+      <c r="C105" s="8"/>
+      <c r="D105" s="8"/>
+      <c r="E105" s="10"/>
+      <c r="F105" s="11"/>
+      <c r="G105" s="15"/>
+      <c r="H105" s="10"/>
+    </row>
+    <row r="106" spans="2:8" ht="18">
+      <c r="B106" s="8"/>
+      <c r="C106" s="8"/>
+      <c r="D106" s="8"/>
+      <c r="E106" s="10"/>
+      <c r="F106" s="11"/>
+      <c r="G106" s="15"/>
+      <c r="H106" s="10"/>
+    </row>
+    <row r="107" spans="2:8" ht="18">
+      <c r="B107" s="8"/>
+      <c r="C107" s="8"/>
+      <c r="D107" s="10"/>
+      <c r="E107" s="10"/>
+      <c r="F107" s="11"/>
+      <c r="G107" s="15"/>
+      <c r="H107" s="10"/>
+    </row>
+    <row r="108" spans="2:8" ht="18">
+      <c r="B108" s="8"/>
+      <c r="C108" s="8"/>
+      <c r="D108" s="10"/>
+      <c r="E108" s="10"/>
+      <c r="F108" s="11"/>
+      <c r="G108" s="15"/>
+      <c r="H108" s="10"/>
+    </row>
+    <row r="109" spans="2:8" ht="18">
+      <c r="B109" s="8"/>
+      <c r="C109" s="8"/>
+      <c r="D109" s="10"/>
+      <c r="E109" s="10"/>
+      <c r="F109" s="11"/>
+      <c r="G109" s="15"/>
+      <c r="H109" s="10"/>
+    </row>
+    <row r="110" spans="2:8" ht="18">
+      <c r="B110" s="8"/>
+      <c r="C110" s="8"/>
+      <c r="D110" s="10"/>
+      <c r="E110" s="10"/>
+      <c r="F110" s="11"/>
+      <c r="G110" s="15"/>
+      <c r="H110" s="10"/>
+    </row>
+    <row r="111" spans="2:8" ht="18">
+      <c r="B111" s="8"/>
+      <c r="C111" s="8"/>
+      <c r="D111" s="10"/>
+      <c r="E111" s="10"/>
+      <c r="F111" s="11"/>
+      <c r="G111" s="15"/>
+      <c r="H111" s="10"/>
+    </row>
+    <row r="112" spans="2:8" ht="18">
+      <c r="B112" s="8"/>
+      <c r="C112" s="8"/>
+      <c r="D112" s="10"/>
+      <c r="E112" s="10"/>
+      <c r="F112" s="11"/>
+      <c r="G112" s="15"/>
+      <c r="H112" s="10"/>
+    </row>
+    <row r="113" spans="2:8" ht="18">
+      <c r="B113" s="8"/>
+      <c r="C113" s="8"/>
+      <c r="D113" s="10"/>
+      <c r="E113" s="10"/>
+      <c r="F113" s="11"/>
+      <c r="G113" s="12"/>
+      <c r="H113" s="10"/>
+    </row>
+    <row r="118" spans="2:8">
+      <c r="C118" s="2"/>
+      <c r="D118"/>
+    </row>
+    <row r="119" spans="2:8">
+      <c r="C119" s="2"/>
+      <c r="D119"/>
+    </row>
+    <row r="120" spans="2:8">
+      <c r="C120" s="2"/>
+      <c r="D120"/>
+    </row>
+    <row r="121" spans="2:8">
+      <c r="C121" s="2"/>
+      <c r="D121"/>
+    </row>
+    <row r="122" spans="2:8">
+      <c r="C122" s="2"/>
+      <c r="D122"/>
+    </row>
+    <row r="123" spans="2:8">
+      <c r="C123" s="2"/>
+      <c r="D123"/>
+    </row>
+    <row r="124" spans="2:8">
+      <c r="C124" s="2"/>
+      <c r="D124"/>
+    </row>
+    <row r="125" spans="2:8">
+      <c r="C125" s="2"/>
+      <c r="D125"/>
+    </row>
+    <row r="126" spans="2:8">
+      <c r="C126" s="2"/>
+      <c r="D126"/>
+    </row>
+    <row r="127" spans="2:8">
+      <c r="C127" s="2"/>
+    </row>
+    <row r="128" spans="2:8">
+      <c r="C128" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
added test_id for each test cases
</commit_message>
<xml_diff>
--- a/Design/Testing_frame_work.xlsx
+++ b/Design/Testing_frame_work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kathe\ITPR7.508-Business-Application-Programming-Semester-One-2024\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5740F4B-94B6-46AB-8671-628F12D27FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D97614-92EB-4CC4-80D6-3E5DC501877F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="176">
   <si>
     <t>Status</t>
   </si>
@@ -498,6 +498,69 @@
   </si>
   <si>
     <t>include tests for valid input data, missing required fields, and invalid data formats.</t>
+  </si>
+  <si>
+    <t>IT_auth_001</t>
+  </si>
+  <si>
+    <t>IT_auth_002</t>
+  </si>
+  <si>
+    <t>IT_auth_003</t>
+  </si>
+  <si>
+    <t>IT_nav_001</t>
+  </si>
+  <si>
+    <t>IT_nav_002</t>
+  </si>
+  <si>
+    <t>IT_form_001</t>
+  </si>
+  <si>
+    <t>IT_form_002</t>
+  </si>
+  <si>
+    <t>IT_form_003</t>
+  </si>
+  <si>
+    <t>IT_form_004</t>
+  </si>
+  <si>
+    <t>IT_performance_001</t>
+  </si>
+  <si>
+    <t>IT_layout_001</t>
+  </si>
+  <si>
+    <t>IT_data_001</t>
+  </si>
+  <si>
+    <t>IT_data_002</t>
+  </si>
+  <si>
+    <t>IT_data_003</t>
+  </si>
+  <si>
+    <t>IT_error_001</t>
+  </si>
+  <si>
+    <t>IT_endpoint_001</t>
+  </si>
+  <si>
+    <t>IT_get_001</t>
+  </si>
+  <si>
+    <t>IT_get_002</t>
+  </si>
+  <si>
+    <t>IT_psot_001</t>
+  </si>
+  <si>
+    <t>IT_put_001</t>
+  </si>
+  <si>
+    <t>IT_delete_001</t>
   </si>
 </sst>
 </file>
@@ -1063,7 +1126,7 @@
   <dimension ref="A1:H128"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A47" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28"/>
+      <selection activeCell="M87" sqref="M87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1916,7 +1979,9 @@
       <c r="D68" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="E68" s="10"/>
+      <c r="E68" s="10" t="s">
+        <v>155</v>
+      </c>
       <c r="F68" s="11"/>
       <c r="G68" s="12"/>
       <c r="H68" s="10"/>
@@ -1927,7 +1992,9 @@
       <c r="D69" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="E69" s="10"/>
+      <c r="E69" s="10" t="s">
+        <v>156</v>
+      </c>
       <c r="F69" s="11"/>
       <c r="G69" s="12"/>
       <c r="H69" s="10"/>
@@ -1938,7 +2005,9 @@
       <c r="D70" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="E70" s="10"/>
+      <c r="E70" s="10" t="s">
+        <v>157</v>
+      </c>
       <c r="F70" s="11"/>
       <c r="G70" s="12"/>
       <c r="H70" s="10"/>
@@ -1960,7 +2029,9 @@
       <c r="D72" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="E72" s="10"/>
+      <c r="E72" s="10" t="s">
+        <v>158</v>
+      </c>
       <c r="F72" s="11"/>
       <c r="G72" s="12"/>
       <c r="H72" s="10"/>
@@ -1971,7 +2042,9 @@
       <c r="D73" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E73" s="10"/>
+      <c r="E73" s="10" t="s">
+        <v>159</v>
+      </c>
       <c r="F73" s="11"/>
       <c r="G73" s="12"/>
       <c r="H73" s="10"/>
@@ -1993,7 +2066,9 @@
       <c r="D75" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="E75" s="10"/>
+      <c r="E75" s="10" t="s">
+        <v>160</v>
+      </c>
       <c r="F75" s="11"/>
       <c r="G75" s="12"/>
       <c r="H75" s="10"/>
@@ -2004,7 +2079,9 @@
       <c r="D76" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="E76" s="10"/>
+      <c r="E76" s="10" t="s">
+        <v>161</v>
+      </c>
       <c r="F76" s="11"/>
       <c r="G76" s="12"/>
       <c r="H76" s="10"/>
@@ -2015,7 +2092,9 @@
       <c r="D77" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="E77" s="10"/>
+      <c r="E77" s="10" t="s">
+        <v>162</v>
+      </c>
       <c r="F77" s="11"/>
       <c r="G77" s="12"/>
       <c r="H77" s="10"/>
@@ -2026,7 +2105,9 @@
       <c r="D78" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="E78" s="10"/>
+      <c r="E78" s="10" t="s">
+        <v>163</v>
+      </c>
       <c r="F78" s="11"/>
       <c r="G78" s="12"/>
       <c r="H78" s="10"/>
@@ -2048,7 +2129,9 @@
       <c r="D80" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="E80" s="10"/>
+      <c r="E80" s="10" t="s">
+        <v>164</v>
+      </c>
       <c r="F80" s="11"/>
       <c r="G80" s="12"/>
       <c r="H80" s="10"/>
@@ -2070,7 +2153,9 @@
       <c r="D82" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="E82" s="10"/>
+      <c r="E82" s="10" t="s">
+        <v>165</v>
+      </c>
       <c r="F82" s="11"/>
       <c r="G82" s="12"/>
       <c r="H82" s="10"/>
@@ -2092,7 +2177,9 @@
       <c r="D84" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="E84" s="10"/>
+      <c r="E84" s="10" t="s">
+        <v>166</v>
+      </c>
       <c r="F84" s="11"/>
       <c r="G84" s="12"/>
       <c r="H84" s="10"/>
@@ -2103,7 +2190,9 @@
       <c r="D85" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="E85" s="10"/>
+      <c r="E85" s="10" t="s">
+        <v>167</v>
+      </c>
       <c r="F85" s="11"/>
       <c r="G85" s="12"/>
       <c r="H85" s="10"/>
@@ -2114,7 +2203,9 @@
       <c r="D86" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="E86" s="10"/>
+      <c r="E86" s="10" t="s">
+        <v>168</v>
+      </c>
       <c r="F86" s="11"/>
       <c r="G86" s="12"/>
       <c r="H86" s="10"/>
@@ -2136,7 +2227,9 @@
       <c r="D88" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="E88" s="10"/>
+      <c r="E88" s="10" t="s">
+        <v>169</v>
+      </c>
       <c r="F88" s="11"/>
       <c r="G88" s="12"/>
       <c r="H88" s="10"/>
@@ -2158,7 +2251,9 @@
       <c r="D90" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="E90" s="10"/>
+      <c r="E90" s="10" t="s">
+        <v>170</v>
+      </c>
       <c r="F90" s="11"/>
       <c r="G90" s="12"/>
       <c r="H90" s="10"/>
@@ -2180,7 +2275,9 @@
       <c r="D92" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="E92" s="10"/>
+      <c r="E92" s="10" t="s">
+        <v>171</v>
+      </c>
       <c r="F92" s="11"/>
       <c r="G92" s="12"/>
       <c r="H92" s="10"/>
@@ -2191,7 +2288,9 @@
       <c r="D93" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="E93" s="10"/>
+      <c r="E93" s="10" t="s">
+        <v>172</v>
+      </c>
       <c r="F93" s="11"/>
       <c r="G93" s="12"/>
       <c r="H93" s="10"/>
@@ -2213,7 +2312,9 @@
       <c r="D95" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="E95" s="10"/>
+      <c r="E95" s="10" t="s">
+        <v>173</v>
+      </c>
       <c r="F95" s="11"/>
       <c r="G95" s="12"/>
       <c r="H95" s="10"/>
@@ -2235,7 +2336,9 @@
       <c r="D97" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="E97" s="10"/>
+      <c r="E97" s="10" t="s">
+        <v>174</v>
+      </c>
       <c r="F97" s="11"/>
       <c r="G97" s="12"/>
       <c r="H97" s="10"/>
@@ -2257,7 +2360,9 @@
       <c r="D99" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="E99" s="10"/>
+      <c r="E99" s="10" t="s">
+        <v>175</v>
+      </c>
       <c r="F99" s="11"/>
       <c r="G99" s="12"/>
       <c r="H99" s="10"/>

</xml_diff>